<commit_message>
reÃparation and improvement done on the get_series function
</commit_message>
<xml_diff>
--- a/time spacing/words/words_V1.0.0.xlsx
+++ b/time spacing/words/words_V1.0.0.xlsx
@@ -2398,9 +2398,6 @@
     <t>question</t>
   </si>
   <si>
-    <t>anser</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -2408,6 +2405,9 @@
   </si>
   <si>
     <t>fr_to_eng</t>
+  </si>
+  <si>
+    <t>answer</t>
   </si>
 </sst>
 </file>
@@ -2746,7 +2746,7 @@
   <dimension ref="A1:E383"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2756,16 +2756,16 @@
         <v>754</v>
       </c>
       <c r="B1" t="s">
+        <v>758</v>
+      </c>
+      <c r="C1" t="s">
         <v>755</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>756</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>757</v>
-      </c>
-      <c r="E1" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="2" spans="1:5">

</xml_diff>